<commit_message>
Diamond cart Code Updated
</commit_message>
<xml_diff>
--- a/src/main/resources/test_data.xlsx
+++ b/src/main/resources/test_data.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>HomePageTitle</t>
   </si>
@@ -61,14 +61,38 @@
     <t>m</t>
   </si>
   <si>
+    <t>MenuOption</t>
+  </si>
+  <si>
     <t xml:space="preserve">
-        </t>
-  </si>
-  <si>
-    <t>Jewelry</t>
-  </si>
-  <si>
-    <t>MenuOption</t>
+  SortOptions     </t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>Name: A to Z</t>
+  </si>
+  <si>
+    <t>Name: Z to A</t>
+  </si>
+  <si>
+    <t>Price: Low to High</t>
+  </si>
+  <si>
+    <t>Black &amp; White Diamond Heart</t>
+  </si>
+  <si>
+    <t>Price: High to Low</t>
+  </si>
+  <si>
+    <t>Created on</t>
+  </si>
+  <si>
+    <t>JEWELRY</t>
+  </si>
+  <si>
+    <t>productName</t>
   </si>
 </sst>
 </file>
@@ -546,29 +570,64 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" customWidth="1"/>
+    <col min="1" max="1" width="17.5546875" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" customWidth="1"/>
+    <col min="3" max="3" width="26.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>15</v>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>